<commit_message>
Folder Re-organization and Updates to medmap and distractmap based on preregistration.
</commit_message>
<xml_diff>
--- a/fMRI Tasks/N-Of-Many/N-of-Many info/biopac_code_dict.xlsx
+++ b/fMRI Tasks/N-Of-Many/N-of-Many info/biopac_code_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\canlab\WASABI_public\fMRI Tasks\N-Of-Many\N-of-Many info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA4B2B9-25B0-47CC-AFA0-C3B07CE0875C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD45007-ECB2-4577-A6D9-041678B6703F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="3285" windowWidth="18240" windowHeight="28440" xr2:uid="{75F97961-46F2-4545-9ED3-F0E6263E2077}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="24312" xr2:uid="{75F97961-46F2-4545-9ED3-F0E6263E2077}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="371">
   <si>
     <t>D8</t>
   </si>
@@ -1141,6 +1141,12 @@
   </si>
   <si>
     <t>nback negative feedback shown</t>
+  </si>
+  <si>
+    <t>expectancy_rating</t>
+  </si>
+  <si>
+    <t>expectancy rating (added for preregistration)</t>
   </si>
 </sst>
 </file>
@@ -1573,7 +1579,7 @@
   <dimension ref="A1:N268"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4036,6 +4042,12 @@
       <c r="M52" s="2"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>370</v>
+      </c>
       <c r="C53" s="2">
         <v>51</v>
       </c>

</xml_diff>